<commit_message>
KeyError 'Events' on page 1 when predicting
</commit_message>
<xml_diff>
--- a/dummy_patient_copy_w_events.xlsx
+++ b/dummy_patient_copy_w_events.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kksta\OneDrive - Northeastern University\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kksta\CapstoneC2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6919CA-EB16-4CF2-B922-713F4AF1499F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC681508-2C2D-4258-BB4F-C7F0A5CE5A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="98">
   <si>
     <t>Record ID</t>
   </si>
@@ -310,6 +310,12 @@
   </si>
   <si>
     <t>Event Type</t>
+  </si>
+  <si>
+    <t>Event reporting 4</t>
+  </si>
+  <si>
+    <t>Thrombotic event not related to the area intervened</t>
   </si>
 </sst>
 </file>
@@ -1332,10 +1338,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5815DC4-32AA-4706-A2C7-746ACE9C7E03}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1354,6 +1360,20 @@
         <v>95</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2">
+        <v>222.43077994188189</v>
+      </c>
+      <c r="D2" t="s">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>